<commit_message>
+ data management section
Signed-off-by: Caleb Grant <geocoug@gmail.com>
</commit_message>
<xml_diff>
--- a/static/resources/workouts.xlsx
+++ b/static/resources/workouts.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgrant/GitHub/geocoug/toolkit/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgrant/GitHub/geocoug/toolkit/static/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FCE1AD-679E-2F46-B1CC-57B519BFC52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319D9523-7C84-6E4F-A7A7-0FBCAC04A347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24280" activeTab="7" xr2:uid="{33B94D11-EE83-ED43-B23D-BCAC305DFE17}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24280" activeTab="3" xr2:uid="{33B94D11-EE83-ED43-B23D-BCAC305DFE17}"/>
   </bookViews>
   <sheets>
     <sheet name="Back-Biceps" sheetId="1" r:id="rId1"/>
     <sheet name="Chest-Triceps" sheetId="2" r:id="rId2"/>
     <sheet name="Legs" sheetId="3" r:id="rId3"/>
     <sheet name="Shoulders-Traps" sheetId="4" r:id="rId4"/>
-    <sheet name="Schedule" sheetId="5" r:id="rId5"/>
-    <sheet name="John-Push" sheetId="6" r:id="rId6"/>
-    <sheet name="John-Pull" sheetId="7" r:id="rId7"/>
-    <sheet name="John-Legs" sheetId="8" r:id="rId8"/>
+    <sheet name="Intro-Push" sheetId="6" r:id="rId5"/>
+    <sheet name="Intro-Pull" sheetId="7" r:id="rId6"/>
+    <sheet name="Intro-Legs" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="105">
   <si>
     <t>Lift</t>
   </si>
@@ -65,9 +64,6 @@
     <t>Lat Pull Downs</t>
   </si>
   <si>
-    <t>Rows</t>
-  </si>
-  <si>
     <t>Dumbbell Rows</t>
   </si>
   <si>
@@ -146,9 +142,6 @@
     <t>Barbell Shrugs</t>
   </si>
   <si>
-    <t>Front Squat</t>
-  </si>
-  <si>
     <t>Ab Roller</t>
   </si>
   <si>
@@ -161,42 +154,6 @@
     <t>Dumbbell Press</t>
   </si>
   <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Cardio</t>
-  </si>
-  <si>
-    <t>Chest &amp; Triceps</t>
-  </si>
-  <si>
-    <t>Legs</t>
-  </si>
-  <si>
-    <t>Shoulders &amp; Traps</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
     <t>How-To</t>
   </si>
   <si>
@@ -242,9 +199,6 @@
     <t>Bird Dog</t>
   </si>
   <si>
-    <t>Leg Kickbacks</t>
-  </si>
-  <si>
     <t>30 seconds</t>
   </si>
   <si>
@@ -263,18 +217,6 @@
     <t>Wipers</t>
   </si>
   <si>
-    <t>Chest &amp; Triceps, Run</t>
-  </si>
-  <si>
-    <t>Back &amp; Biceps</t>
-  </si>
-  <si>
-    <t>Shoulders &amp; Traps, Run</t>
-  </si>
-  <si>
-    <t>Back &amp; Biceps, Run</t>
-  </si>
-  <si>
     <t>Face Pulls</t>
   </si>
   <si>
@@ -336,22 +278,94 @@
   </si>
   <si>
     <t>[View](https://www.verywellfit.com/how-to-do-the-bird-dog-exercise-3498253)</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Pyramid intensity</t>
+  </si>
+  <si>
+    <t>10, 8, 6, 8, 10</t>
+  </si>
+  <si>
+    <t>Rowerg</t>
+  </si>
+  <si>
+    <t>2-5 minutes</t>
+  </si>
+  <si>
+    <t>Warmup</t>
+  </si>
+  <si>
+    <t>Failure on last set</t>
+  </si>
+  <si>
+    <t>Bent Over Rows</t>
+  </si>
+  <si>
+    <t>One Arm Seated Cable Rows</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>6 miles</t>
+  </si>
+  <si>
+    <t>20-30 minutes</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Good Mornings</t>
+  </si>
+  <si>
+    <t>Mixed Cable</t>
+  </si>
+  <si>
+    <t>Leg Curl, Side Step, Knee Raise</t>
+  </si>
+  <si>
+    <t>Hold for 3 seconds at full extension</t>
+  </si>
+  <si>
+    <t>45 seconds</t>
+  </si>
+  <si>
+    <t>5 minutes</t>
+  </si>
+  <si>
+    <t>One Leg Balance</t>
+  </si>
+  <si>
+    <t>On Incline</t>
+  </si>
+  <si>
+    <t>Failure On Last Set</t>
+  </si>
+  <si>
+    <t>Shoulder Superset</t>
+  </si>
+  <si>
+    <t>Dumbell Superset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,12 +408,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,7 +431,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -706,7 +719,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -714,15 +727,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF3C11C-73CE-304C-B13C-F9FD3DC9A2A4}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -732,155 +751,207 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="C12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
         <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4E81E3-F197-394F-B96A-34A73554A4BF}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -890,10 +961,13 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -901,10 +975,13 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -913,9 +990,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -924,20 +1001,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>20</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -946,9 +1023,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -957,9 +1034,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -968,9 +1045,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -979,15 +1056,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10">
         <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -997,15 +1085,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8207F0-C9C2-604E-A375-6CAF3A0DA2A3}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1015,93 +1106,144 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1111,13 +1253,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF8F0F7-407A-0C45-9397-8FA0C20E56A9}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1127,136 +1274,161 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>68</v>
-      </c>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
         <v>20</v>
       </c>
     </row>
@@ -1266,162 +1438,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799A96E5-05A4-0D42-A424-79CE6CD41898}">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66115A2-F7BB-0142-8BE6-1212D3F4745D}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1437,12 +1458,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
@@ -1451,12 +1472,12 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -1465,12 +1486,12 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -1479,12 +1500,12 @@
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -1493,12 +1514,12 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -1507,12 +1528,12 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -1521,26 +1542,26 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2">
         <v>3</v>
@@ -1549,12 +1570,12 @@
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>3</v>
@@ -1562,8 +1583,8 @@
       <c r="C10" s="2">
         <v>10</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>78</v>
+      <c r="D10" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1571,7 +1592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACAA6EF-C076-1A40-B827-2A0EF6A947F7}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1595,12 +1616,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
@@ -1609,12 +1630,12 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -1623,12 +1644,12 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -1637,12 +1658,12 @@
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
       <c r="A5" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -1651,12 +1672,12 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -1665,12 +1686,12 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
       <c r="A7" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -1679,7 +1700,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1687,11 +1708,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA328CD7-D52E-6148-98AF-351AC996FD22}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1708,12 +1729,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2">
         <v>4</v>
@@ -1722,12 +1743,12 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -1736,12 +1757,12 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -1750,24 +1771,24 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="17">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -1776,12 +1797,12 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -1790,7 +1811,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>